<commit_message>
Progresso do desenvolvimento da página de calculadora de fichas
</commit_message>
<xml_diff>
--- a/tags/layout3/doc/Chip Calculator.xlsx
+++ b/tags/layout3/doc/Chip Calculator.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Fichas</t>
   </si>
@@ -32,12 +32,18 @@
   <si>
     <t>média de fichas</t>
   </si>
+  <si>
+    <t>Valor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,13 +74,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -93,7 +92,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="72">
+  <cellStyleXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,15 +165,105 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="72">
+  <cellStyles count="158">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -210,6 +299,49 @@
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -245,6 +377,49 @@
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -575,18 +750,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J2:J7"/>
+    <sheetView tabSelected="1" topLeftCell="O8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -603,11 +779,14 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
       <c r="L1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -615,7 +794,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <f>B$11*B2/100</f>
+        <f>B$9*B2/100</f>
         <v>5000</v>
       </c>
       <c r="D2">
@@ -623,22 +802,25 @@
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>5000</v>
       </c>
       <c r="J2">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K2">
-        <f>J$14*J2/100</f>
-        <v>15000</v>
+        <f>J$11*J2/100</f>
+        <v>4970</v>
       </c>
       <c r="L2">
         <f>K2/I2</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="S2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -646,7 +828,7 @@
         <v>30</v>
       </c>
       <c r="C3">
-        <f>B$11*B3/100</f>
+        <f>B$9*B3/100</f>
         <v>3000</v>
       </c>
       <c r="D3">
@@ -654,22 +836,22 @@
         <v>3</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>1000</v>
       </c>
       <c r="J3">
         <v>15</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K10" si="0">J$14*J3/100</f>
-        <v>3000</v>
+        <f>J$11*J3/100</f>
+        <v>1050</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L10" si="1">K3/I3</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <f t="shared" ref="L3:L8" si="0">K3/I3</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>500</v>
       </c>
@@ -677,30 +859,45 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <f>B$11*B4/100</f>
+        <f>B$9*B4/100</f>
         <v>1000</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D7" si="2">C4/A4</f>
+        <f t="shared" ref="D4:D7" si="1">C4/A4</f>
         <v>2</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>500</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K4">
+        <f>J$11*J4/100</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
         <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>25</v>
+      </c>
+      <c r="S4">
+        <f>R4*2</f>
+        <v>50</v>
+      </c>
+      <c r="T4" s="3">
+        <f>S4*100/S$2</f>
+        <v>0.05</v>
+      </c>
+      <c r="U4" t="str">
+        <f>CONCATENATE(TRUNC(T4,2),",")</f>
+        <v>0,05,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>100</v>
       </c>
@@ -708,30 +905,45 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <f>B$11*B5/100</f>
+        <f>B$9*B5/100</f>
         <v>600</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>600</v>
-      </c>
-      <c r="L5">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="E5" s="1"/>
+      <c r="I5" s="2">
+        <v>100</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <f>J$11*J5/100</f>
+        <v>630</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>6.3</v>
+      </c>
+      <c r="R5">
+        <v>50</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:S33" si="2">R5*2</f>
+        <v>100</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" ref="T5:T33" si="3">S5*100/S$2</f>
+        <v>0.1</v>
+      </c>
+      <c r="U5" t="str">
+        <f t="shared" ref="U5:U33" si="4">CONCATENATE(TRUNC(T5,2),",")</f>
+        <v>0,1,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>50</v>
       </c>
@@ -739,29 +951,44 @@
         <v>2.5</v>
       </c>
       <c r="C6">
-        <f>B$11*B6/100</f>
+        <f>B$9*B6/100</f>
         <v>250</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>50</v>
-      </c>
-      <c r="J6">
-        <v>1.25</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="L6">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="I6" s="2">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f>J$11*J6/100</f>
+        <v>210</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+      <c r="R6">
+        <v>75</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="U6" t="str">
+        <f t="shared" si="4"/>
+        <v>0,15,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>25</v>
       </c>
@@ -769,113 +996,585 @@
         <v>1.5</v>
       </c>
       <c r="C7">
-        <f>B$11*B7/100</f>
+        <f>B$9*B7/100</f>
         <v>150</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>25</v>
-      </c>
-      <c r="J7">
-        <v>0.75</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="L7">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="I8">
-        <v>10</v>
+      <c r="I7" s="2">
+        <v>25</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <f>J$11*J7/100</f>
+        <v>210</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>8.4</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="U7" t="str">
+        <f t="shared" si="4"/>
+        <v>0,2,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v>100</v>
+      </c>
+      <c r="I8" s="2">
+        <v>5</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
+        <f>J$11*J8/100</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>200</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="U8" t="str">
+        <f t="shared" si="4"/>
+        <v>0,4,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="B9">
-        <f>SUM(B2:B7)</f>
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="B11">
         <v>10000</v>
       </c>
-      <c r="C11">
+      <c r="C9">
         <f>SUM(C2:C7)</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="J12">
-        <f>SUM(J2:J10)</f>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>300</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>600</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="U9" t="str">
+        <f t="shared" si="4"/>
+        <v>0,6,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <v>400</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>800</v>
+      </c>
+      <c r="T10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="U10" t="str">
+        <f t="shared" si="4"/>
+        <v>0,8,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="J11">
+        <v>7000</v>
+      </c>
+      <c r="K11">
+        <f>SUM(K2:K8)</f>
+        <v>7070</v>
+      </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <f>AVERAGE(L2:L8)*2</f>
+        <v>5.9840000000000009</v>
+      </c>
+      <c r="Q11">
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <v>500</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="T11" s="3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="U11" t="str">
+        <f t="shared" si="4"/>
+        <v>1,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="Q12">
+        <v>6</v>
+      </c>
+      <c r="R12">
+        <v>600</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>1200</v>
+      </c>
+      <c r="T12" s="3">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
+      </c>
+      <c r="U12" t="str">
+        <f t="shared" si="4"/>
+        <v>1,2,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="Q13">
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <v>700</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>1400</v>
+      </c>
+      <c r="T13" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
+      <c r="U13" t="str">
+        <f t="shared" si="4"/>
+        <v>1,4,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="Q14">
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <v>800</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>1600</v>
+      </c>
+      <c r="T14" s="3">
+        <f t="shared" si="3"/>
+        <v>1.6</v>
+      </c>
+      <c r="U14" t="str">
+        <f t="shared" si="4"/>
+        <v>1,6,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="Q15">
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <v>1000</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>2000</v>
+      </c>
+      <c r="T15" s="3">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="U15" t="str">
+        <f t="shared" si="4"/>
+        <v>2,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="Q16">
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <v>1200</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>2400</v>
+      </c>
+      <c r="T16" s="3">
+        <f t="shared" si="3"/>
+        <v>2.4</v>
+      </c>
+      <c r="U16" t="str">
+        <f t="shared" si="4"/>
+        <v>2,4,</v>
+      </c>
+    </row>
+    <row r="17" spans="17:21">
+      <c r="Q17">
+        <v>11</v>
+      </c>
+      <c r="R17">
+        <v>1400</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>2800</v>
+      </c>
+      <c r="T17" s="3">
+        <f t="shared" si="3"/>
+        <v>2.8</v>
+      </c>
+      <c r="U17" t="str">
+        <f t="shared" si="4"/>
+        <v>2,8,</v>
+      </c>
+    </row>
+    <row r="18" spans="17:21">
+      <c r="Q18">
+        <v>12</v>
+      </c>
+      <c r="R18">
+        <v>1800</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>3600</v>
+      </c>
+      <c r="T18" s="3">
+        <f t="shared" si="3"/>
+        <v>3.6</v>
+      </c>
+      <c r="U18" t="str">
+        <f t="shared" si="4"/>
+        <v>3,6,</v>
+      </c>
+    </row>
+    <row r="19" spans="17:21">
+      <c r="Q19">
+        <v>13</v>
+      </c>
+      <c r="R19">
+        <v>2000</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>4000</v>
+      </c>
+      <c r="T19" s="3">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U19" t="str">
+        <f t="shared" si="4"/>
+        <v>4,</v>
+      </c>
+    </row>
+    <row r="20" spans="17:21">
+      <c r="Q20">
+        <v>14</v>
+      </c>
+      <c r="R20">
+        <v>2500</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>5000</v>
+      </c>
+      <c r="T20" s="3">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U20" t="str">
+        <f t="shared" si="4"/>
+        <v>5,</v>
+      </c>
+    </row>
+    <row r="21" spans="17:21">
+      <c r="Q21">
+        <v>15</v>
+      </c>
+      <c r="R21">
+        <v>3000</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>6000</v>
+      </c>
+      <c r="T21" s="3">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U21" t="str">
+        <f t="shared" si="4"/>
+        <v>6,</v>
+      </c>
+    </row>
+    <row r="22" spans="17:21">
+      <c r="Q22">
+        <v>16</v>
+      </c>
+      <c r="R22">
+        <v>3500</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>7000</v>
+      </c>
+      <c r="T22" s="3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U22" t="str">
+        <f t="shared" si="4"/>
+        <v>7,</v>
+      </c>
+    </row>
+    <row r="23" spans="17:21">
+      <c r="Q23">
+        <v>17</v>
+      </c>
+      <c r="R23">
+        <v>4000</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="2"/>
+        <v>8000</v>
+      </c>
+      <c r="T23" s="3">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" si="4"/>
+        <v>8,</v>
+      </c>
+    </row>
+    <row r="24" spans="17:21">
+      <c r="Q24">
+        <v>18</v>
+      </c>
+      <c r="R24">
+        <v>5000</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="4"/>
+        <v>10,</v>
+      </c>
+    </row>
+    <row r="25" spans="17:21">
+      <c r="Q25">
+        <v>19</v>
+      </c>
+      <c r="R25">
+        <v>6000</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>12000</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="4"/>
+        <v>12,</v>
+      </c>
+    </row>
+    <row r="26" spans="17:21">
+      <c r="Q26">
+        <v>20</v>
+      </c>
+      <c r="R26">
+        <v>7500</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="2"/>
+        <v>15000</v>
+      </c>
+      <c r="T26" s="3">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="4"/>
+        <v>15,</v>
+      </c>
+    </row>
+    <row r="27" spans="17:21">
+      <c r="Q27">
+        <v>21</v>
+      </c>
+      <c r="R27">
+        <v>10000</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="T27" s="3">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="4"/>
+        <v>20,</v>
+      </c>
+    </row>
+    <row r="28" spans="17:21">
+      <c r="R28">
+        <v>15000</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="2"/>
+        <v>30000</v>
+      </c>
+      <c r="T28" s="3">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="4"/>
+        <v>30,</v>
+      </c>
+    </row>
+    <row r="29" spans="17:21">
+      <c r="R29">
+        <v>20000</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="T29" s="3">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="4"/>
+        <v>40,</v>
+      </c>
+    </row>
+    <row r="30" spans="17:21">
+      <c r="R30">
+        <v>25000</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+      <c r="T30" s="3">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="4"/>
+        <v>50,</v>
+      </c>
+    </row>
+    <row r="31" spans="17:21">
+      <c r="R31">
+        <v>30000</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="2"/>
+        <v>60000</v>
+      </c>
+      <c r="T31" s="3">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="4"/>
+        <v>60,</v>
+      </c>
+    </row>
+    <row r="32" spans="17:21">
+      <c r="R32">
+        <v>40000</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="2"/>
+        <v>80000</v>
+      </c>
+      <c r="T32" s="3">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="4"/>
+        <v>80,</v>
+      </c>
+    </row>
+    <row r="33" spans="18:21">
+      <c r="R33">
+        <v>50000</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>100000</v>
+      </c>
+      <c r="T33" s="3">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="J14">
-        <v>20000</v>
-      </c>
-      <c r="K14">
-        <f>SUM(K2:K10)</f>
-        <v>20000</v>
-      </c>
-      <c r="M14" t="s">
-        <v>3</v>
-      </c>
-      <c r="N14">
-        <f>AVERAGE(L2:L10)*2</f>
-        <v>5.5555555555555554</v>
+      <c r="U33" t="str">
+        <f t="shared" si="4"/>
+        <v>100,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>